<commit_message>
Convert gambar dan split data train test
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -5,22 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KULIAH\Document\Semester 7\Machine Learning\Prak\Project_ML_158_147\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69278B86-7F75-47E3-812F-DF2BA6853D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DB3CCB-32E9-4015-86BC-A87EB155B90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -37,27 +46,12 @@
     <t>Pre processing</t>
   </si>
   <si>
-    <t>20 Oktober 2021</t>
-  </si>
-  <si>
-    <t>- selection format image</t>
-  </si>
-  <si>
-    <t>- resizing</t>
-  </si>
-  <si>
-    <t>- splitting</t>
-  </si>
-  <si>
     <t>Modelling CNN</t>
   </si>
   <si>
     <t>24 Oktober 2021</t>
   </si>
   <si>
-    <t>- Modelling CNN (vgg16)</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -76,15 +70,6 @@
     <t>testing</t>
   </si>
   <si>
-    <t>18 Oktober 2021</t>
-  </si>
-  <si>
-    <t>22 Oktober 2021</t>
-  </si>
-  <si>
-    <t>26 Oktober 2021</t>
-  </si>
-  <si>
     <t>02 November 2021</t>
   </si>
   <si>
@@ -92,13 +77,28 @@
   </si>
   <si>
     <t>Dina</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>On Going</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>19 Oktober 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -115,6 +115,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,7 +130,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -147,24 +153,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -173,6 +180,10 @@
     </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,204 +402,153 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="10"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>